<commit_message>
Changed batch labels on ALL data set
</commit_message>
<xml_diff>
--- a/output/all_planning.xlsx
+++ b/output/all_planning.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LR\WLR\Documents-\WangLR\University\Y2S1\URECA\Code\testingPackage3\output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LR\WLR\Documents-\WangLR\University\Y2S1\URECA\Code\doppelgangerSpotting\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF057F30-C4DD-4206-B61C-5F55C181C72D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D46E4C89-5BF2-44E5-ADDA-C46FF5ADDDD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,241 +37,241 @@
     <t>Class</t>
   </si>
   <si>
-    <t>BCR_1_A</t>
-  </si>
-  <si>
-    <t>A</t>
+    <t>BCR_1_R</t>
+  </si>
+  <si>
+    <t>R</t>
   </si>
   <si>
     <t>BCR</t>
   </si>
   <si>
-    <t>BCR_2_A</t>
-  </si>
-  <si>
-    <t>BCR_3_A</t>
-  </si>
-  <si>
-    <t>BCR_4_A</t>
-  </si>
-  <si>
-    <t>BCR_5_A</t>
-  </si>
-  <si>
-    <t>BCR_6_A</t>
-  </si>
-  <si>
-    <t>BCR_7_A</t>
-  </si>
-  <si>
-    <t>BCR_8_A</t>
-  </si>
-  <si>
-    <t>BCR_9_A</t>
-  </si>
-  <si>
-    <t>BCR_10_A</t>
-  </si>
-  <si>
-    <t>BCR_11_A</t>
-  </si>
-  <si>
-    <t>BCR_12_A</t>
-  </si>
-  <si>
-    <t>BCR_13_A</t>
-  </si>
-  <si>
-    <t>BCR_14_A</t>
-  </si>
-  <si>
-    <t>BCR_15_A</t>
-  </si>
-  <si>
-    <t>E2A_1_A</t>
+    <t>BCR_2_R</t>
+  </si>
+  <si>
+    <t>BCR_3_R</t>
+  </si>
+  <si>
+    <t>BCR_4_R</t>
+  </si>
+  <si>
+    <t>BCR_5_R</t>
+  </si>
+  <si>
+    <t>BCR_6_R</t>
+  </si>
+  <si>
+    <t>BCR_7_R</t>
+  </si>
+  <si>
+    <t>BCR_8_R</t>
+  </si>
+  <si>
+    <t>BCR_9_R</t>
+  </si>
+  <si>
+    <t>BCR_10_R</t>
+  </si>
+  <si>
+    <t>BCR_11_R</t>
+  </si>
+  <si>
+    <t>BCR_12_R</t>
+  </si>
+  <si>
+    <t>BCR_13_R</t>
+  </si>
+  <si>
+    <t>BCR_14_R</t>
+  </si>
+  <si>
+    <t>BCR_15_R</t>
+  </si>
+  <si>
+    <t>E2A_1_R</t>
   </si>
   <si>
     <t>E2A</t>
   </si>
   <si>
-    <t>E2A_2_A</t>
-  </si>
-  <si>
-    <t>E2A_3_A</t>
-  </si>
-  <si>
-    <t>E2A_4_A</t>
-  </si>
-  <si>
-    <t>E2A_5_A</t>
-  </si>
-  <si>
-    <t>E2A_6_A</t>
-  </si>
-  <si>
-    <t>E2A_7_A</t>
-  </si>
-  <si>
-    <t>E2A_8_A</t>
-  </si>
-  <si>
-    <t>E2A_9_A</t>
-  </si>
-  <si>
-    <t>E2A_10_A</t>
-  </si>
-  <si>
-    <t>E2A_11_A</t>
-  </si>
-  <si>
-    <t>E2A_12_A</t>
-  </si>
-  <si>
-    <t>E2A_13_A</t>
-  </si>
-  <si>
-    <t>E2A_14_A</t>
-  </si>
-  <si>
-    <t>E2A_15_A</t>
-  </si>
-  <si>
-    <t>E2A_16_A</t>
-  </si>
-  <si>
-    <t>E2A_17_A</t>
-  </si>
-  <si>
-    <t>E2A_18_A</t>
-  </si>
-  <si>
-    <t>BCR_1_M</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>BCR_2_M</t>
-  </si>
-  <si>
-    <t>BCR_3_M</t>
-  </si>
-  <si>
-    <t>BCR_4_M</t>
-  </si>
-  <si>
-    <t>BCR_5_M</t>
-  </si>
-  <si>
-    <t>BCR_6_M</t>
-  </si>
-  <si>
-    <t>BCR_7_M</t>
-  </si>
-  <si>
-    <t>BCR_8_M</t>
-  </si>
-  <si>
-    <t>BCR_9_M</t>
-  </si>
-  <si>
-    <t>BCR_10_M</t>
-  </si>
-  <si>
-    <t>BCR_11_M</t>
-  </si>
-  <si>
-    <t>BCR_12_M</t>
-  </si>
-  <si>
-    <t>BCR_13_M</t>
-  </si>
-  <si>
-    <t>BCR_14_M</t>
-  </si>
-  <si>
-    <t>BCR_15_M</t>
-  </si>
-  <si>
-    <t>E2A_1_M</t>
-  </si>
-  <si>
-    <t>E2A_2_M</t>
-  </si>
-  <si>
-    <t>E2A_3_M</t>
-  </si>
-  <si>
-    <t>E2A_4_M</t>
-  </si>
-  <si>
-    <t>E2A_5_M</t>
-  </si>
-  <si>
-    <t>E2A_6_M</t>
-  </si>
-  <si>
-    <t>E2A_7_M</t>
-  </si>
-  <si>
-    <t>E2A_8_M</t>
-  </si>
-  <si>
-    <t>E2A_9_M</t>
-  </si>
-  <si>
-    <t>E2A_10_M</t>
-  </si>
-  <si>
-    <t>E2A_11_M</t>
-  </si>
-  <si>
-    <t>E2A_12_M</t>
-  </si>
-  <si>
-    <t>E2A_13_M</t>
-  </si>
-  <si>
-    <t>E2A_14_M</t>
-  </si>
-  <si>
-    <t>E2A_15_M</t>
-  </si>
-  <si>
-    <t>E2A_16_M</t>
-  </si>
-  <si>
-    <t>E2A_17_M</t>
-  </si>
-  <si>
-    <t>E2A_18_M</t>
-  </si>
-  <si>
-    <t>E2A_19_M</t>
-  </si>
-  <si>
-    <t>E2A_20_M</t>
-  </si>
-  <si>
-    <t>E2A_21_M</t>
-  </si>
-  <si>
-    <t>E2A_22_M</t>
-  </si>
-  <si>
-    <t>E2A_23_M</t>
-  </si>
-  <si>
-    <t>E2A_24_M</t>
-  </si>
-  <si>
-    <t>E2A_25_M</t>
-  </si>
-  <si>
-    <t>E2A_26_M</t>
-  </si>
-  <si>
-    <t>E2A_27_M</t>
+    <t>E2A_2_R</t>
+  </si>
+  <si>
+    <t>E2A_3_R</t>
+  </si>
+  <si>
+    <t>E2A_4_R</t>
+  </si>
+  <si>
+    <t>E2A_5_R</t>
+  </si>
+  <si>
+    <t>E2A_6_R</t>
+  </si>
+  <si>
+    <t>E2A_7_R</t>
+  </si>
+  <si>
+    <t>E2A_8_R</t>
+  </si>
+  <si>
+    <t>E2A_9_R</t>
+  </si>
+  <si>
+    <t>E2A_10_R</t>
+  </si>
+  <si>
+    <t>E2A_11_R</t>
+  </si>
+  <si>
+    <t>E2A_12_R</t>
+  </si>
+  <si>
+    <t>E2A_13_R</t>
+  </si>
+  <si>
+    <t>E2A_14_R</t>
+  </si>
+  <si>
+    <t>E2A_15_R</t>
+  </si>
+  <si>
+    <t>E2A_16_R</t>
+  </si>
+  <si>
+    <t>E2A_17_R</t>
+  </si>
+  <si>
+    <t>E2A_18_R</t>
+  </si>
+  <si>
+    <t>BCR_1_Y</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>BCR_2_Y</t>
+  </si>
+  <si>
+    <t>BCR_3_Y</t>
+  </si>
+  <si>
+    <t>BCR_4_Y</t>
+  </si>
+  <si>
+    <t>BCR_5_Y</t>
+  </si>
+  <si>
+    <t>BCR_6_Y</t>
+  </si>
+  <si>
+    <t>BCR_7_Y</t>
+  </si>
+  <si>
+    <t>BCR_8_Y</t>
+  </si>
+  <si>
+    <t>BCR_9_Y</t>
+  </si>
+  <si>
+    <t>BCR_10_Y</t>
+  </si>
+  <si>
+    <t>BCR_11_Y</t>
+  </si>
+  <si>
+    <t>BCR_12_Y</t>
+  </si>
+  <si>
+    <t>BCR_13_Y</t>
+  </si>
+  <si>
+    <t>BCR_14_Y</t>
+  </si>
+  <si>
+    <t>BCR_15_Y</t>
+  </si>
+  <si>
+    <t>E2A_1_Y</t>
+  </si>
+  <si>
+    <t>E2A_2_Y</t>
+  </si>
+  <si>
+    <t>E2A_3_Y</t>
+  </si>
+  <si>
+    <t>E2A_4_Y</t>
+  </si>
+  <si>
+    <t>E2A_5_Y</t>
+  </si>
+  <si>
+    <t>E2A_6_Y</t>
+  </si>
+  <si>
+    <t>E2A_7_Y</t>
+  </si>
+  <si>
+    <t>E2A_8_Y</t>
+  </si>
+  <si>
+    <t>E2A_9_Y</t>
+  </si>
+  <si>
+    <t>E2A_10_Y</t>
+  </si>
+  <si>
+    <t>E2A_11_Y</t>
+  </si>
+  <si>
+    <t>E2A_12_Y</t>
+  </si>
+  <si>
+    <t>E2A_13_Y</t>
+  </si>
+  <si>
+    <t>E2A_14_Y</t>
+  </si>
+  <si>
+    <t>E2A_15_Y</t>
+  </si>
+  <si>
+    <t>E2A_16_Y</t>
+  </si>
+  <si>
+    <t>E2A_17_Y</t>
+  </si>
+  <si>
+    <t>E2A_18_Y</t>
+  </si>
+  <si>
+    <t>E2A_19_Y</t>
+  </si>
+  <si>
+    <t>E2A_20_Y</t>
+  </si>
+  <si>
+    <t>E2A_21_Y</t>
+  </si>
+  <si>
+    <t>E2A_22_Y</t>
+  </si>
+  <si>
+    <t>E2A_23_Y</t>
+  </si>
+  <si>
+    <t>E2A_24_Y</t>
+  </si>
+  <si>
+    <t>E2A_25_Y</t>
+  </si>
+  <si>
+    <t>E2A_26_Y</t>
+  </si>
+  <si>
+    <t>E2A_27_Y</t>
   </si>
   <si>
     <t>Sample1</t>
@@ -308,16 +308,16 @@
     <t>Doppel_0.valid</t>
   </si>
   <si>
+    <t>Doppel_1_Unbal.train</t>
+  </si>
+  <si>
+    <t>Doppel_1_Unbal.valid</t>
+  </si>
+  <si>
     <t>Doppel_1.train</t>
   </si>
   <si>
     <t>Doppel_1.valid</t>
-  </si>
-  <si>
-    <t>Doppel_1_Unbal.train</t>
-  </si>
-  <si>
-    <t>Doppel_1_Unbal.valid</t>
   </si>
   <si>
     <t>Doppel_2.train</t>
@@ -354,7 +354,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -376,26 +376,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -410,16 +397,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -718,8 +699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C76"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50:A64"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1570,9 +1551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <sheetData>
@@ -1594,7 +1573,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A2" s="4" t="s">
+      <c r="A2" t="s">
         <v>25</v>
       </c>
       <c r="B2" t="s">
@@ -1705,48 +1684,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
-  <cols>
-    <col min="1" max="3" width="10.90625" style="1"/>
-    <col min="4" max="4" width="24.76953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.453125" style="1" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>84</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>85</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
         <v>0.975749794763763</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>87</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1760,18 +1732,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
-  <cols>
-    <col min="1" max="1" width="7.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.76953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.453125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
@@ -1818,173 +1781,173 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="19.36328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.90625" style="2"/>
+    <col min="2" max="2" width="10.90625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.75">
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.75">
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.75">
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.75">
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.75">
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.75">
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.75">
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.75">
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.75">
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.75">
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.75">
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.75">
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="1" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1998,7 +1961,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <sheetData>
@@ -2225,20 +2188,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ABD8AB7-64E2-4BC6-9939-F8E63D70AC69}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2B24B84-B5B9-436A-9B55-9301A8C1B302}">
   <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
-  <cols>
-    <col min="1" max="2" width="12.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="18.6796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="15" width="12.86328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.04296875" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
@@ -2248,16 +2205,16 @@
         <v>92</v>
       </c>
       <c r="C1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" t="s">
         <v>95</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>96</v>
-      </c>
-      <c r="E1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F1" t="s">
-        <v>94</v>
       </c>
       <c r="G1" t="s">
         <v>97</v>
@@ -2294,49 +2251,49 @@
       <c r="A2" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
       <c r="E2" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" t="s">
         <v>3</v>
       </c>
       <c r="G2" t="s">
         <v>39</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" t="s">
         <v>3</v>
       </c>
       <c r="I2" t="s">
         <v>39</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" t="s">
         <v>3</v>
       </c>
       <c r="K2" t="s">
         <v>39</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" t="s">
         <v>3</v>
       </c>
       <c r="M2" t="s">
         <v>39</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" t="s">
         <v>3</v>
       </c>
       <c r="O2" t="s">
         <v>39</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2344,49 +2301,49 @@
       <c r="A3" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" t="s">
         <v>6</v>
       </c>
       <c r="E3" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" t="s">
         <v>6</v>
       </c>
       <c r="G3" t="s">
         <v>41</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" t="s">
         <v>6</v>
       </c>
       <c r="I3" t="s">
         <v>41</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" t="s">
         <v>6</v>
       </c>
       <c r="K3" t="s">
         <v>41</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="L3" t="s">
         <v>6</v>
       </c>
       <c r="M3" t="s">
         <v>41</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="N3" t="s">
         <v>6</v>
       </c>
       <c r="O3" t="s">
         <v>41</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="P3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2394,49 +2351,49 @@
       <c r="A4" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" t="s">
         <v>7</v>
       </c>
       <c r="E4" t="s">
         <v>42</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" t="s">
         <v>7</v>
       </c>
       <c r="G4" t="s">
         <v>42</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" t="s">
         <v>7</v>
       </c>
       <c r="I4" t="s">
         <v>42</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" t="s">
         <v>7</v>
       </c>
       <c r="K4" t="s">
         <v>42</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="L4" t="s">
         <v>7</v>
       </c>
       <c r="M4" t="s">
         <v>42</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="N4" t="s">
         <v>7</v>
       </c>
       <c r="O4" t="s">
         <v>42</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="P4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2444,49 +2401,49 @@
       <c r="A5" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="C5" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" t="s">
         <v>8</v>
       </c>
       <c r="E5" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" t="s">
         <v>8</v>
       </c>
       <c r="G5" t="s">
         <v>43</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" t="s">
         <v>8</v>
       </c>
       <c r="I5" t="s">
         <v>43</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" t="s">
         <v>8</v>
       </c>
       <c r="K5" t="s">
         <v>43</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="L5" t="s">
         <v>8</v>
       </c>
       <c r="M5" t="s">
         <v>43</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="N5" t="s">
         <v>8</v>
       </c>
       <c r="O5" t="s">
         <v>43</v>
       </c>
-      <c r="P5" s="2" t="s">
+      <c r="P5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2494,49 +2451,49 @@
       <c r="A6" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" t="s">
         <v>9</v>
       </c>
       <c r="E6" t="s">
         <v>44</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" t="s">
         <v>9</v>
       </c>
       <c r="G6" t="s">
         <v>44</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" t="s">
         <v>9</v>
       </c>
       <c r="I6" t="s">
         <v>44</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J6" t="s">
         <v>9</v>
       </c>
       <c r="K6" t="s">
         <v>44</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="L6" t="s">
         <v>9</v>
       </c>
       <c r="M6" t="s">
         <v>44</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="N6" t="s">
         <v>9</v>
       </c>
       <c r="O6" t="s">
         <v>44</v>
       </c>
-      <c r="P6" s="2" t="s">
+      <c r="P6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2544,43 +2501,43 @@
       <c r="A7" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" t="s">
         <v>20</v>
       </c>
       <c r="C7" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" t="s">
         <v>22</v>
       </c>
       <c r="E7" t="s">
         <v>45</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" t="s">
         <v>25</v>
       </c>
       <c r="G7" t="s">
         <v>45</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" t="s">
         <v>25</v>
       </c>
       <c r="I7" t="s">
         <v>45</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="J7" t="s">
         <v>25</v>
       </c>
       <c r="K7" t="s">
         <v>45</v>
       </c>
-      <c r="L7" s="6" t="s">
+      <c r="L7" t="s">
         <v>25</v>
       </c>
       <c r="M7" t="s">
         <v>45</v>
       </c>
-      <c r="N7" s="6" t="s">
+      <c r="N7" t="s">
         <v>25</v>
       </c>
       <c r="O7" t="s">
@@ -2594,43 +2551,43 @@
       <c r="A8" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" t="s">
         <v>23</v>
       </c>
       <c r="C8" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" t="s">
         <v>23</v>
       </c>
       <c r="E8" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" t="s">
         <v>23</v>
       </c>
       <c r="G8" t="s">
         <v>46</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" t="s">
         <v>27</v>
       </c>
       <c r="I8" t="s">
         <v>46</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="J8" t="s">
         <v>27</v>
       </c>
       <c r="K8" t="s">
         <v>46</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="L8" t="s">
         <v>27</v>
       </c>
       <c r="M8" t="s">
         <v>46</v>
       </c>
-      <c r="N8" s="3" t="s">
+      <c r="N8" t="s">
         <v>27</v>
       </c>
       <c r="O8" t="s">
@@ -2644,43 +2601,43 @@
       <c r="A9" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" t="s">
         <v>24</v>
       </c>
       <c r="C9" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" t="s">
         <v>24</v>
       </c>
       <c r="E9" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" t="s">
         <v>24</v>
       </c>
       <c r="G9" t="s">
         <v>47</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" t="s">
         <v>24</v>
       </c>
       <c r="I9" t="s">
         <v>47</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="J9" t="s">
         <v>32</v>
       </c>
       <c r="K9" t="s">
         <v>47</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="L9" t="s">
         <v>32</v>
       </c>
       <c r="M9" t="s">
         <v>47</v>
       </c>
-      <c r="N9" s="3" t="s">
+      <c r="N9" t="s">
         <v>32</v>
       </c>
       <c r="O9" t="s">
@@ -2694,43 +2651,43 @@
       <c r="A10" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" t="s">
         <v>26</v>
       </c>
       <c r="C10" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" t="s">
         <v>26</v>
       </c>
       <c r="E10" t="s">
         <v>48</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" t="s">
         <v>26</v>
       </c>
       <c r="G10" t="s">
         <v>48</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" t="s">
         <v>26</v>
       </c>
       <c r="I10" t="s">
         <v>48</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="J10" t="s">
         <v>26</v>
       </c>
       <c r="K10" t="s">
         <v>48</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="L10" t="s">
         <v>34</v>
       </c>
       <c r="M10" t="s">
         <v>48</v>
       </c>
-      <c r="N10" s="3" t="s">
+      <c r="N10" t="s">
         <v>34</v>
       </c>
       <c r="O10" t="s">
@@ -2744,43 +2701,43 @@
       <c r="A11" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" t="s">
         <v>28</v>
       </c>
       <c r="C11" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" t="s">
         <v>28</v>
       </c>
       <c r="E11" t="s">
         <v>49</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" t="s">
         <v>28</v>
       </c>
       <c r="G11" t="s">
         <v>49</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" t="s">
         <v>28</v>
       </c>
       <c r="I11" t="s">
         <v>49</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="J11" t="s">
         <v>28</v>
       </c>
       <c r="K11" t="s">
         <v>49</v>
       </c>
-      <c r="L11" s="2" t="s">
+      <c r="L11" t="s">
         <v>28</v>
       </c>
       <c r="M11" t="s">
         <v>49</v>
       </c>
-      <c r="N11" s="3" t="s">
+      <c r="N11" t="s">
         <v>35</v>
       </c>
       <c r="O11" t="s">

</xml_diff>